<commit_message>
Latest version with 1000 chosen apostles + latest untitled and preprocessing
</commit_message>
<xml_diff>
--- a/Faculty.xlsx
+++ b/Faculty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthur\git\ns-project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769EADD5-6C67-4BCD-A0F2-F6DE385D3B04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E502CE-9BFF-4C78-A804-8EC6BADF6AEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11746" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7155" yWindow="0" windowWidth="12045" windowHeight="11550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="by course" sheetId="2" r:id="rId1"/>

</xml_diff>